<commit_message>
update data emisi jabar.
</commit_message>
<xml_diff>
--- a/Jabar/Data Jabar/Emisi/Data Emisi Jabar.xlsx
+++ b/Jabar/Data Jabar/Emisi/Data Emisi Jabar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\System Dynamics\system_dynamics_reference\Jabar\Data Jabar\Emisi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB7E974-0BA6-4AF3-87F1-1203726DE0D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A12487C-4714-44F7-A679-A860BCFE84C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="30" yWindow="30" windowWidth="20460" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7995" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Emisi Energi" sheetId="1" r:id="rId1"/>
@@ -2844,14 +2844,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2871,30 +2892,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2904,11 +2913,101 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2946,102 +3045,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3054,18 +3057,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3073,24 +3091,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3375,8 +3375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:M27"/>
+    <sheetView topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3397,18 +3397,18 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
@@ -3420,21 +3420,21 @@
       <c r="A5" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="99" t="s">
+      <c r="B5" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="99" t="s">
+      <c r="C5" s="107"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="100"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="102" t="s">
+      <c r="F5" s="107"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="103"/>
-      <c r="J5" s="104"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="111"/>
       <c r="K5" s="97" t="s">
         <v>4</v>
       </c>
@@ -3469,10 +3469,10 @@
         <v>12</v>
       </c>
       <c r="K6" s="98"/>
-      <c r="L6" s="178" t="s">
+      <c r="L6" s="96" t="s">
         <v>255</v>
       </c>
-      <c r="M6" s="178" t="s">
+      <c r="M6" s="96" t="s">
         <v>256</v>
       </c>
     </row>
@@ -4424,24 +4424,24 @@
       <c r="K29" s="10"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="105" t="s">
+      <c r="A30" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="105"/>
-      <c r="C30" s="105"/>
-      <c r="D30" s="105"/>
-      <c r="E30" s="105"/>
+      <c r="B30" s="99"/>
+      <c r="C30" s="99"/>
+      <c r="D30" s="99"/>
+      <c r="E30" s="99"/>
     </row>
     <row r="33" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="96" t="s">
+      <c r="A33" s="100" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="96"/>
-      <c r="C33" s="96"/>
-      <c r="D33" s="96"/>
-      <c r="E33" s="96"/>
-      <c r="F33" s="96"/>
-      <c r="G33" s="96"/>
+      <c r="B33" s="100"/>
+      <c r="C33" s="100"/>
+      <c r="D33" s="100"/>
+      <c r="E33" s="100"/>
+      <c r="F33" s="100"/>
+      <c r="G33" s="100"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
@@ -4450,17 +4450,17 @@
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="109" t="s">
+      <c r="A36" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="106" t="s">
+      <c r="B36" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="107"/>
-      <c r="D36" s="108"/>
+      <c r="C36" s="102"/>
+      <c r="D36" s="103"/>
     </row>
     <row r="37" spans="1:7" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="110"/>
+      <c r="A37" s="105"/>
       <c r="B37" s="18" t="s">
         <v>20</v>
       </c>
@@ -4959,27 +4959,27 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="96"/>
-      <c r="B62" s="96"/>
-      <c r="C62" s="96"/>
-      <c r="D62" s="96"/>
-      <c r="E62" s="96"/>
-      <c r="F62" s="96"/>
-      <c r="G62" s="96"/>
+      <c r="A62" s="100"/>
+      <c r="B62" s="100"/>
+      <c r="C62" s="100"/>
+      <c r="D62" s="100"/>
+      <c r="E62" s="100"/>
+      <c r="F62" s="100"/>
+      <c r="G62" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="A62:G62"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5010,22 +5010,22 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="111" t="s">
+      <c r="B3" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="113" t="s">
+      <c r="C3" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="115"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="118"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="112"/>
-      <c r="B4" s="112"/>
+      <c r="A4" s="113"/>
+      <c r="B4" s="113"/>
       <c r="C4" s="30" t="s">
         <v>40</v>
       </c>
@@ -5146,22 +5146,22 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="111" t="s">
+      <c r="A17" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="116" t="s">
+      <c r="B17" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="113" t="s">
+      <c r="C17" s="116" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="114"/>
-      <c r="E17" s="114"/>
-      <c r="F17" s="115"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="118"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="112"/>
-      <c r="B18" s="117"/>
+      <c r="A18" s="113"/>
+      <c r="B18" s="115"/>
       <c r="C18" s="30" t="s">
         <v>40</v>
       </c>
@@ -5722,22 +5722,22 @@
     </row>
     <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="111" t="s">
+      <c r="A50" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="B50" s="116" t="s">
+      <c r="B50" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="113" t="s">
+      <c r="C50" s="116" t="s">
         <v>83</v>
       </c>
-      <c r="D50" s="114"/>
-      <c r="E50" s="114"/>
-      <c r="F50" s="115"/>
+      <c r="D50" s="117"/>
+      <c r="E50" s="117"/>
+      <c r="F50" s="118"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="112"/>
-      <c r="B51" s="117"/>
+      <c r="A51" s="113"/>
+      <c r="B51" s="115"/>
       <c r="C51" s="30" t="s">
         <v>40</v>
       </c>
@@ -6271,7 +6271,7 @@
         <v>27948.078000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="20">
         <v>27</v>
       </c>
@@ -6298,22 +6298,22 @@
     </row>
     <row r="82" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="83" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="111" t="s">
+      <c r="A83" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="B83" s="111" t="s">
+      <c r="B83" s="112" t="s">
         <v>53</v>
       </c>
-      <c r="C83" s="113" t="s">
+      <c r="C83" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="D83" s="114"/>
-      <c r="E83" s="114"/>
-      <c r="F83" s="115"/>
+      <c r="D83" s="117"/>
+      <c r="E83" s="117"/>
+      <c r="F83" s="118"/>
     </row>
     <row r="84" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="112"/>
-      <c r="B84" s="112"/>
+      <c r="A84" s="113"/>
+      <c r="B84" s="113"/>
       <c r="C84" s="30" t="s">
         <v>40</v>
       </c>
@@ -7155,18 +7155,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:F17"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="C50:F50"/>
     <mergeCell ref="A83:A84"/>
     <mergeCell ref="B83:B84"/>
     <mergeCell ref="C83:F83"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7211,18 +7211,18 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="121" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="124" t="s">
+      <c r="A5" s="154" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="157" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="125"/>
-      <c r="D5" s="125"/>
-      <c r="E5" s="126"/>
+      <c r="C5" s="158"/>
+      <c r="D5" s="158"/>
+      <c r="E5" s="159"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="122"/>
+      <c r="A6" s="155"/>
       <c r="B6" s="45" t="s">
         <v>113</v>
       </c>
@@ -7232,18 +7232,18 @@
       <c r="D6" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="121" t="s">
+      <c r="E6" s="154" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="123"/>
-      <c r="B7" s="127" t="s">
+      <c r="A7" s="156"/>
+      <c r="B7" s="160" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="128"/>
-      <c r="D7" s="129"/>
-      <c r="E7" s="123"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="156"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
@@ -7682,7 +7682,7 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="109" t="s">
+      <c r="A37" s="104" t="s">
         <v>0</v>
       </c>
       <c r="B37" s="17" t="s">
@@ -7696,7 +7696,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="110"/>
+      <c r="A38" s="105"/>
       <c r="B38" s="18" t="s">
         <v>122</v>
       </c>
@@ -8100,30 +8100,30 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="118" t="s">
+      <c r="A67" s="151" t="s">
         <v>115</v>
       </c>
-      <c r="B67" s="119"/>
-      <c r="C67" s="120"/>
+      <c r="B67" s="152"/>
+      <c r="C67" s="153"/>
       <c r="D67" s="44">
         <v>8712.44</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="105" t="s">
+      <c r="A68" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="B68" s="105"/>
-      <c r="C68" s="105"/>
-      <c r="D68" s="105"/>
+      <c r="B68" s="99"/>
+      <c r="C68" s="99"/>
+      <c r="D68" s="99"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="130" t="s">
+      <c r="A69" s="150" t="s">
         <v>125</v>
       </c>
-      <c r="B69" s="130"/>
-      <c r="C69" s="130"/>
-      <c r="D69" s="130"/>
+      <c r="B69" s="150"/>
+      <c r="C69" s="150"/>
+      <c r="D69" s="150"/>
     </row>
     <row r="72" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A72" s="28" t="s">
@@ -8137,27 +8137,27 @@
     </row>
     <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="131" t="s">
+      <c r="A75" s="137" t="s">
         <v>19</v>
       </c>
-      <c r="B75" s="133" t="s">
+      <c r="B75" s="146" t="s">
         <v>127</v>
       </c>
-      <c r="C75" s="134"/>
-      <c r="D75" s="133" t="s">
+      <c r="C75" s="147"/>
+      <c r="D75" s="146" t="s">
         <v>128</v>
       </c>
-      <c r="E75" s="134"/>
-      <c r="F75" s="133" t="s">
+      <c r="E75" s="147"/>
+      <c r="F75" s="146" t="s">
         <v>129</v>
       </c>
-      <c r="G75" s="134"/>
-      <c r="H75" s="131" t="s">
+      <c r="G75" s="147"/>
+      <c r="H75" s="137" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="132"/>
+      <c r="A76" s="138"/>
       <c r="B76" s="52" t="s">
         <v>131</v>
       </c>
@@ -8176,7 +8176,7 @@
       <c r="G76" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="H76" s="132"/>
+      <c r="H76" s="138"/>
     </row>
     <row r="77" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="53">
@@ -8861,31 +8861,31 @@
     </row>
     <row r="110" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="111" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="131" t="s">
+      <c r="A111" s="137" t="s">
         <v>19</v>
       </c>
-      <c r="B111" s="133" t="s">
+      <c r="B111" s="146" t="s">
         <v>127</v>
       </c>
-      <c r="C111" s="134"/>
-      <c r="D111" s="133" t="s">
+      <c r="C111" s="147"/>
+      <c r="D111" s="146" t="s">
         <v>128</v>
       </c>
-      <c r="E111" s="134"/>
-      <c r="F111" s="133" t="s">
+      <c r="E111" s="147"/>
+      <c r="F111" s="146" t="s">
         <v>129</v>
       </c>
-      <c r="G111" s="134"/>
-      <c r="H111" s="135" t="s">
+      <c r="G111" s="147"/>
+      <c r="H111" s="148" t="s">
         <v>139</v>
       </c>
-      <c r="I111" s="136"/>
-      <c r="J111" s="131" t="s">
+      <c r="I111" s="149"/>
+      <c r="J111" s="137" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="112" spans="1:10" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="132"/>
+      <c r="A112" s="138"/>
       <c r="B112" s="52" t="s">
         <v>140</v>
       </c>
@@ -8910,7 +8910,7 @@
       <c r="I112" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="J112" s="132"/>
+      <c r="J112" s="138"/>
     </row>
     <row r="113" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
@@ -9665,29 +9665,29 @@
     </row>
     <row r="142" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A143" s="137" t="s">
+      <c r="A143" s="139" t="s">
         <v>19</v>
       </c>
-      <c r="B143" s="140" t="s">
+      <c r="B143" s="142" t="s">
         <v>144</v>
       </c>
-      <c r="C143" s="141"/>
-      <c r="D143" s="140" t="s">
+      <c r="C143" s="143"/>
+      <c r="D143" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="E143" s="141"/>
+      <c r="E143" s="143"/>
     </row>
     <row r="144" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="138"/>
-      <c r="B144" s="142" t="s">
+      <c r="A144" s="140"/>
+      <c r="B144" s="144" t="s">
         <v>145</v>
       </c>
-      <c r="C144" s="143"/>
-      <c r="D144" s="142"/>
-      <c r="E144" s="143"/>
+      <c r="C144" s="145"/>
+      <c r="D144" s="144"/>
+      <c r="E144" s="145"/>
     </row>
     <row r="145" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="139"/>
+      <c r="A145" s="141"/>
       <c r="B145" s="54" t="s">
         <v>146</v>
       </c>
@@ -10148,23 +10148,23 @@
     </row>
     <row r="177" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="178" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="109" t="s">
+      <c r="A178" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="B178" s="145" t="s">
+      <c r="B178" s="134" t="s">
         <v>156</v>
       </c>
-      <c r="C178" s="146"/>
-      <c r="D178" s="145" t="s">
+      <c r="C178" s="135"/>
+      <c r="D178" s="134" t="s">
         <v>157</v>
       </c>
-      <c r="E178" s="147"/>
+      <c r="E178" s="136"/>
       <c r="F178" s="61" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="144"/>
+      <c r="A179" s="133"/>
       <c r="B179" s="19" t="s">
         <v>159</v>
       </c>
@@ -10688,30 +10688,30 @@
     </row>
     <row r="208" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="209" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="148" t="s">
+      <c r="A209" s="122" t="s">
         <v>162</v>
       </c>
-      <c r="B209" s="148" t="s">
+      <c r="B209" s="122" t="s">
         <v>163</v>
       </c>
-      <c r="C209" s="150" t="s">
+      <c r="C209" s="127" t="s">
         <v>164</v>
       </c>
-      <c r="D209" s="151"/>
-      <c r="E209" s="151"/>
-      <c r="F209" s="151"/>
-      <c r="G209" s="151"/>
-      <c r="H209" s="151"/>
-      <c r="I209" s="151"/>
-      <c r="J209" s="151"/>
-      <c r="K209" s="151"/>
-      <c r="L209" s="151"/>
-      <c r="M209" s="151"/>
-      <c r="N209" s="152"/>
+      <c r="D209" s="128"/>
+      <c r="E209" s="128"/>
+      <c r="F209" s="128"/>
+      <c r="G209" s="128"/>
+      <c r="H209" s="128"/>
+      <c r="I209" s="128"/>
+      <c r="J209" s="128"/>
+      <c r="K209" s="128"/>
+      <c r="L209" s="128"/>
+      <c r="M209" s="128"/>
+      <c r="N209" s="132"/>
     </row>
     <row r="210" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="149"/>
-      <c r="B210" s="149"/>
+      <c r="A210" s="123"/>
+      <c r="B210" s="123"/>
       <c r="C210" s="63">
         <v>2008</v>
       </c>
@@ -10881,7 +10881,7 @@
         <v>113157</v>
       </c>
     </row>
-    <row r="214" spans="1:14" ht="40.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="79" t="s">
         <v>169</v>
       </c>
@@ -11058,30 +11058,30 @@
       </c>
     </row>
     <row r="218" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A218" s="148" t="s">
+      <c r="A218" s="122" t="s">
         <v>162</v>
       </c>
-      <c r="B218" s="148" t="s">
+      <c r="B218" s="122" t="s">
         <v>163</v>
       </c>
-      <c r="C218" s="150" t="s">
+      <c r="C218" s="127" t="s">
         <v>189</v>
       </c>
-      <c r="D218" s="151"/>
-      <c r="E218" s="151"/>
-      <c r="F218" s="151"/>
-      <c r="G218" s="151"/>
-      <c r="H218" s="151"/>
-      <c r="I218" s="151"/>
-      <c r="J218" s="151"/>
-      <c r="K218" s="151"/>
-      <c r="L218" s="151"/>
-      <c r="M218" s="153"/>
+      <c r="D218" s="128"/>
+      <c r="E218" s="128"/>
+      <c r="F218" s="128"/>
+      <c r="G218" s="128"/>
+      <c r="H218" s="128"/>
+      <c r="I218" s="128"/>
+      <c r="J218" s="128"/>
+      <c r="K218" s="128"/>
+      <c r="L218" s="128"/>
+      <c r="M218" s="129"/>
       <c r="N218" s="70"/>
     </row>
     <row r="219" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="149"/>
-      <c r="B219" s="149"/>
+      <c r="A219" s="123"/>
+      <c r="B219" s="123"/>
       <c r="C219" s="63">
         <v>2020</v>
       </c>
@@ -11243,7 +11243,7 @@
       </c>
       <c r="N222" s="74"/>
     </row>
-    <row r="223" spans="1:14" ht="40.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="79" t="s">
         <v>169</v>
       </c>
@@ -11412,30 +11412,30 @@
       <c r="N226" s="74"/>
     </row>
     <row r="227" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A227" s="154" t="s">
+      <c r="A227" s="130" t="s">
         <v>194</v>
       </c>
-      <c r="B227" s="148" t="s">
+      <c r="B227" s="122" t="s">
         <v>195</v>
       </c>
-      <c r="C227" s="150" t="s">
+      <c r="C227" s="127" t="s">
         <v>196</v>
       </c>
-      <c r="D227" s="151"/>
-      <c r="E227" s="151"/>
-      <c r="F227" s="151"/>
-      <c r="G227" s="151"/>
-      <c r="H227" s="151"/>
-      <c r="I227" s="151"/>
-      <c r="J227" s="151"/>
-      <c r="K227" s="151"/>
-      <c r="L227" s="151"/>
-      <c r="M227" s="151"/>
-      <c r="N227" s="152"/>
+      <c r="D227" s="128"/>
+      <c r="E227" s="128"/>
+      <c r="F227" s="128"/>
+      <c r="G227" s="128"/>
+      <c r="H227" s="128"/>
+      <c r="I227" s="128"/>
+      <c r="J227" s="128"/>
+      <c r="K227" s="128"/>
+      <c r="L227" s="128"/>
+      <c r="M227" s="128"/>
+      <c r="N227" s="132"/>
     </row>
     <row r="228" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="155"/>
-      <c r="B228" s="149"/>
+      <c r="A228" s="131"/>
+      <c r="B228" s="123"/>
       <c r="C228" s="63">
         <v>2008</v>
       </c>
@@ -11477,7 +11477,7 @@
       <c r="A229" s="79" t="s">
         <v>165</v>
       </c>
-      <c r="B229" s="156" t="s">
+      <c r="B229" s="119" t="s">
         <v>197</v>
       </c>
       <c r="C229" s="80">
@@ -11521,7 +11521,7 @@
       <c r="A230" s="79" t="s">
         <v>167</v>
       </c>
-      <c r="B230" s="157"/>
+      <c r="B230" s="120"/>
       <c r="C230" s="80">
         <v>98.62</v>
       </c>
@@ -11563,7 +11563,7 @@
       <c r="A231" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="B231" s="157"/>
+      <c r="B231" s="120"/>
       <c r="C231" s="82">
         <v>1535.38</v>
       </c>
@@ -11601,11 +11601,11 @@
         <v>2376.31</v>
       </c>
     </row>
-    <row r="232" spans="1:14" ht="40.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="79" t="s">
         <v>169</v>
       </c>
-      <c r="B232" s="157"/>
+      <c r="B232" s="120"/>
       <c r="C232" s="80">
         <v>25.7</v>
       </c>
@@ -11647,7 +11647,7 @@
       <c r="A233" s="79" t="s">
         <v>173</v>
       </c>
-      <c r="B233" s="157"/>
+      <c r="B233" s="120"/>
       <c r="C233" s="80">
         <v>0.14000000000000001</v>
       </c>
@@ -11689,7 +11689,7 @@
       <c r="A234" s="79" t="s">
         <v>175</v>
       </c>
-      <c r="B234" s="157"/>
+      <c r="B234" s="120"/>
       <c r="C234" s="80">
         <v>609.03</v>
       </c>
@@ -11731,7 +11731,7 @@
       <c r="A235" s="79" t="s">
         <v>177</v>
       </c>
-      <c r="B235" s="157"/>
+      <c r="B235" s="120"/>
       <c r="C235" s="80">
         <v>1.1499999999999999</v>
       </c>
@@ -11773,7 +11773,7 @@
       <c r="A236" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="B236" s="158"/>
+      <c r="B236" s="121"/>
       <c r="C236" s="85">
         <v>3060.87</v>
       </c>
@@ -11812,30 +11812,30 @@
       </c>
     </row>
     <row r="237" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A237" s="148" t="s">
+      <c r="A237" s="122" t="s">
         <v>162</v>
       </c>
-      <c r="B237" s="148" t="s">
+      <c r="B237" s="122" t="s">
         <v>195</v>
       </c>
-      <c r="C237" s="159" t="s">
+      <c r="C237" s="124" t="s">
         <v>196</v>
       </c>
-      <c r="D237" s="160"/>
-      <c r="E237" s="160"/>
-      <c r="F237" s="160"/>
-      <c r="G237" s="160"/>
-      <c r="H237" s="160"/>
-      <c r="I237" s="160"/>
-      <c r="J237" s="160"/>
-      <c r="K237" s="160"/>
-      <c r="L237" s="160"/>
-      <c r="M237" s="161"/>
+      <c r="D237" s="125"/>
+      <c r="E237" s="125"/>
+      <c r="F237" s="125"/>
+      <c r="G237" s="125"/>
+      <c r="H237" s="125"/>
+      <c r="I237" s="125"/>
+      <c r="J237" s="125"/>
+      <c r="K237" s="125"/>
+      <c r="L237" s="125"/>
+      <c r="M237" s="126"/>
       <c r="N237" s="70"/>
     </row>
     <row r="238" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A238" s="149"/>
-      <c r="B238" s="149"/>
+      <c r="A238" s="123"/>
+      <c r="B238" s="123"/>
       <c r="C238" s="63">
         <v>2020</v>
       </c>
@@ -11875,7 +11875,7 @@
       <c r="A239" s="79" t="s">
         <v>165</v>
       </c>
-      <c r="B239" s="156" t="s">
+      <c r="B239" s="119" t="s">
         <v>197</v>
       </c>
       <c r="C239" s="80">
@@ -11917,7 +11917,7 @@
       <c r="A240" s="79" t="s">
         <v>167</v>
       </c>
-      <c r="B240" s="157"/>
+      <c r="B240" s="120"/>
       <c r="C240" s="80">
         <v>91.29</v>
       </c>
@@ -11957,7 +11957,7 @@
       <c r="A241" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="B241" s="157"/>
+      <c r="B241" s="120"/>
       <c r="C241" s="82">
         <v>2453.83</v>
       </c>
@@ -11993,11 +11993,11 @@
       </c>
       <c r="N241" s="74"/>
     </row>
-    <row r="242" spans="1:14" ht="40.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:14" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="79" t="s">
         <v>169</v>
       </c>
-      <c r="B242" s="157"/>
+      <c r="B242" s="120"/>
       <c r="C242" s="80">
         <v>43.65</v>
       </c>
@@ -12037,7 +12037,7 @@
       <c r="A243" s="79" t="s">
         <v>173</v>
       </c>
-      <c r="B243" s="157"/>
+      <c r="B243" s="120"/>
       <c r="C243" s="80">
         <v>0.39</v>
       </c>
@@ -12077,7 +12077,7 @@
       <c r="A244" s="79" t="s">
         <v>175</v>
       </c>
-      <c r="B244" s="157"/>
+      <c r="B244" s="120"/>
       <c r="C244" s="82">
         <v>1977.75</v>
       </c>
@@ -12117,7 +12117,7 @@
       <c r="A245" s="79" t="s">
         <v>177</v>
       </c>
-      <c r="B245" s="157"/>
+      <c r="B245" s="120"/>
       <c r="C245" s="80">
         <v>21.77</v>
       </c>
@@ -12157,7 +12157,7 @@
       <c r="A246" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="B246" s="158"/>
+      <c r="B246" s="121"/>
       <c r="C246" s="85">
         <v>5386.45</v>
       </c>
@@ -12195,28 +12195,17 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B229:B236"/>
-    <mergeCell ref="A237:A238"/>
-    <mergeCell ref="B237:B238"/>
-    <mergeCell ref="C237:M237"/>
-    <mergeCell ref="B239:B246"/>
-    <mergeCell ref="A218:A219"/>
-    <mergeCell ref="B218:B219"/>
-    <mergeCell ref="C218:M218"/>
-    <mergeCell ref="A227:A228"/>
-    <mergeCell ref="B227:B228"/>
-    <mergeCell ref="C227:N227"/>
-    <mergeCell ref="A178:A179"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="D178:E178"/>
-    <mergeCell ref="A209:A210"/>
-    <mergeCell ref="B209:B210"/>
-    <mergeCell ref="C209:N209"/>
-    <mergeCell ref="J111:J112"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="D143:E144"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="D75:E75"/>
     <mergeCell ref="H75:H76"/>
     <mergeCell ref="A111:A112"/>
     <mergeCell ref="B111:C111"/>
@@ -12224,17 +12213,28 @@
     <mergeCell ref="F111:G111"/>
     <mergeCell ref="H111:I111"/>
     <mergeCell ref="F75:G75"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="J111:J112"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="D143:E144"/>
+    <mergeCell ref="A178:A179"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="D178:E178"/>
+    <mergeCell ref="A209:A210"/>
+    <mergeCell ref="B209:B210"/>
+    <mergeCell ref="C209:N209"/>
+    <mergeCell ref="A218:A219"/>
+    <mergeCell ref="B218:B219"/>
+    <mergeCell ref="C218:M218"/>
+    <mergeCell ref="A227:A228"/>
+    <mergeCell ref="B227:B228"/>
+    <mergeCell ref="C227:N227"/>
+    <mergeCell ref="B229:B236"/>
+    <mergeCell ref="A237:A238"/>
+    <mergeCell ref="B237:B238"/>
+    <mergeCell ref="C237:M237"/>
+    <mergeCell ref="B239:B246"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12244,8 +12244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12272,17 +12272,17 @@
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24"/>
-      <c r="B5" s="133" t="s">
+      <c r="B5" s="146" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="164"/>
-      <c r="D5" s="134"/>
-      <c r="E5" s="133" t="s">
+      <c r="C5" s="165"/>
+      <c r="D5" s="147"/>
+      <c r="E5" s="146" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="164"/>
-      <c r="G5" s="134"/>
-      <c r="H5" s="131" t="s">
+      <c r="F5" s="165"/>
+      <c r="G5" s="147"/>
+      <c r="H5" s="137" t="s">
         <v>36</v>
       </c>
     </row>
@@ -12308,7 +12308,7 @@
       <c r="G6" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="132"/>
+      <c r="H6" s="138"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20">
@@ -12857,7 +12857,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="162" t="s">
+      <c r="A28" s="163" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="27">
@@ -12873,7 +12873,7 @@
       <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="163"/>
+      <c r="A29" s="164"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="27">
@@ -12889,16 +12889,16 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="165" t="s">
+      <c r="A30" s="166" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="165"/>
-      <c r="C30" s="165"/>
-      <c r="D30" s="165"/>
-      <c r="E30" s="165"/>
-      <c r="F30" s="165"/>
-      <c r="G30" s="165"/>
-      <c r="H30" s="165"/>
+      <c r="B30" s="166"/>
+      <c r="C30" s="166"/>
+      <c r="D30" s="166"/>
+      <c r="E30" s="166"/>
+      <c r="F30" s="166"/>
+      <c r="G30" s="166"/>
+      <c r="H30" s="166"/>
       <c r="I30" s="91"/>
       <c r="J30" s="91"/>
     </row>
@@ -12944,16 +12944,16 @@
       <c r="A3" s="13"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="100" t="s">
         <v>217</v>
       </c>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
@@ -12965,24 +12965,24 @@
       <c r="A7" s="167" t="s">
         <v>204</v>
       </c>
-      <c r="B7" s="170" t="s">
+      <c r="B7" s="176" t="s">
         <v>205</v>
       </c>
-      <c r="C7" s="171"/>
-      <c r="D7" s="171"/>
-      <c r="E7" s="171"/>
-      <c r="F7" s="171"/>
-      <c r="G7" s="171"/>
-      <c r="H7" s="171"/>
-      <c r="I7" s="171"/>
-      <c r="J7" s="172"/>
-      <c r="K7" s="173" t="s">
+      <c r="C7" s="177"/>
+      <c r="D7" s="177"/>
+      <c r="E7" s="177"/>
+      <c r="F7" s="177"/>
+      <c r="G7" s="177"/>
+      <c r="H7" s="177"/>
+      <c r="I7" s="177"/>
+      <c r="J7" s="178"/>
+      <c r="K7" s="171" t="s">
         <v>206</v>
       </c>
-      <c r="L7" s="174"/>
+      <c r="L7" s="172"/>
     </row>
     <row r="8" spans="1:12" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="169"/>
+      <c r="A8" s="170"/>
       <c r="B8" s="92" t="s">
         <v>207</v>
       </c>
@@ -13010,8 +13010,8 @@
       <c r="J8" s="92" t="s">
         <v>214</v>
       </c>
-      <c r="K8" s="175"/>
-      <c r="L8" s="176"/>
+      <c r="K8" s="173"/>
+      <c r="L8" s="174"/>
     </row>
     <row r="9" spans="1:12" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="168"/>
@@ -13848,12 +13848,12 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="96" t="s">
+      <c r="A33" s="100" t="s">
         <v>218</v>
       </c>
-      <c r="B33" s="96"/>
-      <c r="C33" s="96"/>
-      <c r="D33" s="96"/>
+      <c r="B33" s="100"/>
+      <c r="C33" s="100"/>
+      <c r="D33" s="100"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
@@ -13861,20 +13861,20 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="109" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="106" t="s">
+      <c r="A35" s="104" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="101" t="s">
         <v>220</v>
       </c>
-      <c r="C35" s="107"/>
-      <c r="D35" s="107"/>
-      <c r="E35" s="107"/>
-      <c r="F35" s="107"/>
-      <c r="G35" s="108"/>
+      <c r="C35" s="102"/>
+      <c r="D35" s="102"/>
+      <c r="E35" s="102"/>
+      <c r="F35" s="102"/>
+      <c r="G35" s="103"/>
     </row>
     <row r="36" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="166"/>
+      <c r="A36" s="175"/>
       <c r="B36" s="18" t="s">
         <v>221</v>
       </c>
@@ -13891,7 +13891,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="110"/>
+      <c r="A37" s="105"/>
       <c r="B37" s="19" t="s">
         <v>215</v>
       </c>
@@ -14410,33 +14410,33 @@
     </row>
     <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="109" t="s">
-        <v>0</v>
-      </c>
-      <c r="B64" s="106" t="s">
+      <c r="A64" s="104" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="101" t="s">
         <v>230</v>
       </c>
-      <c r="C64" s="107"/>
-      <c r="D64" s="107"/>
-      <c r="E64" s="107"/>
-      <c r="F64" s="108"/>
+      <c r="C64" s="102"/>
+      <c r="D64" s="102"/>
+      <c r="E64" s="102"/>
+      <c r="F64" s="103"/>
     </row>
     <row r="65" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="166"/>
-      <c r="B65" s="106" t="s">
+      <c r="A65" s="175"/>
+      <c r="B65" s="101" t="s">
         <v>221</v>
       </c>
-      <c r="C65" s="108"/>
-      <c r="D65" s="106" t="s">
+      <c r="C65" s="103"/>
+      <c r="D65" s="101" t="s">
         <v>222</v>
       </c>
-      <c r="E65" s="108"/>
+      <c r="E65" s="103"/>
       <c r="F65" s="167" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="110"/>
+      <c r="A66" s="105"/>
       <c r="B66" s="19" t="s">
         <v>231</v>
       </c>
@@ -14891,12 +14891,12 @@
       <c r="A92" s="167" t="s">
         <v>0</v>
       </c>
-      <c r="B92" s="106" t="s">
+      <c r="B92" s="101" t="s">
         <v>235</v>
       </c>
-      <c r="C92" s="107"/>
-      <c r="D92" s="107"/>
-      <c r="E92" s="177"/>
+      <c r="C92" s="102"/>
+      <c r="D92" s="102"/>
+      <c r="E92" s="169"/>
     </row>
     <row r="93" spans="1:7" ht="186" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="168"/>
@@ -15285,10 +15285,10 @@
       <c r="A120" s="167" t="s">
         <v>0</v>
       </c>
-      <c r="B120" s="106" t="s">
+      <c r="B120" s="101" t="s">
         <v>221</v>
       </c>
-      <c r="C120" s="108"/>
+      <c r="C120" s="103"/>
       <c r="D120" s="17" t="s">
         <v>222</v>
       </c>
@@ -15298,7 +15298,7 @@
       </c>
     </row>
     <row r="121" spans="1:6" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="169"/>
+      <c r="A121" s="170"/>
       <c r="B121" s="19" t="s">
         <v>231</v>
       </c>
@@ -15316,7 +15316,7 @@
       </c>
     </row>
     <row r="122" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="169"/>
+      <c r="A122" s="170"/>
       <c r="B122" s="167" t="s">
         <v>242</v>
       </c>
@@ -16095,13 +16095,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:E92"/>
-    <mergeCell ref="A120:A123"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="D122:D123"/>
     <mergeCell ref="K7:L8"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A33:D33"/>
@@ -16115,6 +16108,13 @@
     <mergeCell ref="G36:G37"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:J7"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:E92"/>
+    <mergeCell ref="A120:A123"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="D122:D123"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16124,8 +16124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>